<commit_message>
Overview Of Group Functions
</commit_message>
<xml_diff>
--- a/9.Group-Functions/Group-Functions.xlsx
+++ b/9.Group-Functions/Group-Functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\oracle\9.Group-Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C69EFBD-BF52-4922-A658-9654DD90B0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA4957F-8FFA-489C-9C6C-769ACEBE28AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29250" yWindow="300" windowWidth="24900" windowHeight="13320" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29250" yWindow="300" windowWidth="24900" windowHeight="13320" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group Functions" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="MIN Function" sheetId="5" r:id="rId5"/>
     <sheet name="SUM Function" sheetId="6" r:id="rId6"/>
     <sheet name="LISTAGG Function" sheetId="7" r:id="rId7"/>
+    <sheet name="Overview Of Group Functions" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="118">
   <si>
     <t>oracle</t>
     <phoneticPr fontId="1"/>
@@ -1358,6 +1359,115 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> in one column, and the list of the emplyees having that job title are returned in the other column</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7.Overview+of+Group+Functions+(Code+Samples).sql</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>oracle\9.Group-Functions\7.Overview+of+Group+Functions+(Code+Samples).sql</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t> * Lecture : Overview of Group Functions                    *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT SUM(salary), AVG(salary), MAX(hire_date), MIN(commission_pct), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT(DISTINCT manager_id), LISTAGG(job_id,',') </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">COUNT(DISTINCT manager_id), LISTAGG(job_id,','), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hire_date</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">in a query, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all the columns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> must be within a group function. If not we get an error</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If we write a column name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>without a group function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. For example </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hire_date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> we will get an error. So if we write a group function</t>
     </r>
     <phoneticPr fontId="1"/>
   </si>
@@ -1530,9 +1640,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3603,6 +3713,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>522521</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{265C89AD-6117-F191-C360-0565416AB4A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="4962525"/>
+          <a:ext cx="10895246" cy="5149850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>61790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17901681-F3BE-4507-E9D3-2134C78B9676}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="15182850"/>
+          <a:ext cx="11391900" cy="2481140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5736,8 +5939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E89431-25B7-4E20-8BCD-454FC2B8E48B}">
   <dimension ref="B3:U275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="V266" sqref="V266"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -5852,7 +6055,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="4"/>
-      <c r="D17" s="11" t="s">
+      <c r="D17" t="s">
         <v>62</v>
       </c>
       <c r="M17" s="5"/>
@@ -5903,538 +6106,188 @@
       <c r="B39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
       <c r="M39" s="5"/>
     </row>
     <row r="40" spans="2:13">
       <c r="B40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
       <c r="M40" s="5"/>
     </row>
     <row r="41" spans="2:13">
       <c r="B41" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
       <c r="M41" s="5"/>
     </row>
     <row r="42" spans="2:13">
       <c r="B42" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
       <c r="M42" s="5"/>
     </row>
     <row r="43" spans="2:13">
       <c r="B43" s="4"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
       <c r="M43" s="5"/>
     </row>
     <row r="44" spans="2:13">
       <c r="B44" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
       <c r="M44" s="5"/>
     </row>
     <row r="45" spans="2:13">
       <c r="B45" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
       <c r="M45" s="5"/>
     </row>
     <row r="46" spans="2:13">
       <c r="B46" s="4"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="12"/>
       <c r="M46" s="5"/>
     </row>
     <row r="47" spans="2:13">
       <c r="B47" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="12"/>
       <c r="M47" s="5"/>
     </row>
     <row r="48" spans="2:13">
       <c r="B48" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="12"/>
       <c r="M48" s="5"/>
     </row>
     <row r="49" spans="2:13">
       <c r="B49" s="4"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="12"/>
-      <c r="L49" s="12"/>
       <c r="M49" s="5"/>
     </row>
     <row r="50" spans="2:13">
       <c r="B50" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
       <c r="M50" s="5"/>
     </row>
     <row r="51" spans="2:13">
       <c r="B51" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="12"/>
       <c r="M51" s="5"/>
     </row>
     <row r="52" spans="2:13">
       <c r="B52" s="4"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="12"/>
       <c r="M52" s="5"/>
     </row>
     <row r="53" spans="2:13">
       <c r="B53" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
       <c r="M53" s="5"/>
     </row>
     <row r="54" spans="2:13">
       <c r="B54" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
       <c r="M54" s="5"/>
     </row>
     <row r="55" spans="2:13">
       <c r="B55" s="4"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
       <c r="M55" s="5"/>
     </row>
     <row r="56" spans="2:13">
       <c r="B56" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
       <c r="M56" s="5"/>
     </row>
     <row r="57" spans="2:13">
       <c r="B57" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="12"/>
       <c r="M57" s="5"/>
     </row>
     <row r="58" spans="2:13">
       <c r="B58" s="4"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
-      <c r="K58" s="12"/>
-      <c r="L58" s="12"/>
       <c r="M58" s="5"/>
     </row>
     <row r="59" spans="2:13">
       <c r="B59" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-      <c r="K59" s="12"/>
-      <c r="L59" s="12"/>
       <c r="M59" s="5"/>
     </row>
     <row r="60" spans="2:13">
       <c r="B60" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-      <c r="K60" s="12"/>
-      <c r="L60" s="12"/>
       <c r="M60" s="5"/>
     </row>
     <row r="61" spans="2:13">
       <c r="B61" s="4"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="12"/>
-      <c r="L61" s="12"/>
       <c r="M61" s="5"/>
     </row>
     <row r="62" spans="2:13">
       <c r="B62" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="12"/>
-      <c r="L62" s="12"/>
       <c r="M62" s="5"/>
     </row>
     <row r="63" spans="2:13">
       <c r="B63" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
-      <c r="L63" s="12"/>
       <c r="M63" s="5"/>
     </row>
     <row r="64" spans="2:13">
       <c r="B64" s="4"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12"/>
       <c r="M64" s="5"/>
     </row>
     <row r="65" spans="2:15">
       <c r="B65" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12"/>
       <c r="M65" s="5"/>
     </row>
     <row r="66" spans="2:15">
       <c r="B66" s="4"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="12"/>
-      <c r="J66" s="12"/>
-      <c r="K66" s="12"/>
-      <c r="L66" s="12"/>
       <c r="M66" s="5"/>
     </row>
     <row r="67" spans="2:15">
       <c r="B67" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="12"/>
-      <c r="K67" s="12"/>
-      <c r="L67" s="12"/>
       <c r="M67" s="5"/>
     </row>
     <row r="68" spans="2:15">
       <c r="B68" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
       <c r="M68" s="5"/>
     </row>
     <row r="69" spans="2:15">
       <c r="B69" s="4"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="12"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="12"/>
-      <c r="K69" s="12"/>
-      <c r="L69" s="12"/>
       <c r="M69" s="5"/>
     </row>
     <row r="70" spans="2:15">
       <c r="B70" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="12"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="12"/>
-      <c r="K70" s="12"/>
-      <c r="L70" s="12"/>
       <c r="M70" s="5"/>
     </row>
     <row r="71" spans="2:15">
       <c r="B71" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="12"/>
-      <c r="K71" s="12"/>
-      <c r="L71" s="12"/>
       <c r="M71" s="5"/>
     </row>
     <row r="72" spans="2:15">
       <c r="B72" s="4"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="12"/>
-      <c r="K72" s="12"/>
-      <c r="L72" s="12"/>
       <c r="M72" s="5"/>
     </row>
     <row r="73" spans="2:15">
       <c r="B73" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="12"/>
-      <c r="K73" s="12"/>
-      <c r="L73" s="12"/>
       <c r="M73" s="5"/>
       <c r="N73" t="s">
         <v>23</v>
@@ -6447,202 +6300,72 @@
       <c r="B74" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="12"/>
-      <c r="K74" s="12"/>
-      <c r="L74" s="12"/>
       <c r="M74" s="5"/>
     </row>
     <row r="75" spans="2:15">
       <c r="B75" s="4"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="12"/>
-      <c r="K75" s="12"/>
-      <c r="L75" s="12"/>
       <c r="M75" s="5"/>
     </row>
     <row r="76" spans="2:15">
       <c r="B76" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
-      <c r="J76" s="12"/>
-      <c r="K76" s="12"/>
-      <c r="L76" s="12"/>
       <c r="M76" s="5"/>
     </row>
     <row r="77" spans="2:15">
       <c r="B77" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="12"/>
-      <c r="K77" s="12"/>
-      <c r="L77" s="12"/>
       <c r="M77" s="5"/>
     </row>
     <row r="78" spans="2:15">
       <c r="B78" s="4"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
-      <c r="K78" s="12"/>
-      <c r="L78" s="12"/>
       <c r="M78" s="5"/>
     </row>
     <row r="79" spans="2:15">
       <c r="B79" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
-      <c r="K79" s="12"/>
-      <c r="L79" s="12"/>
       <c r="M79" s="5"/>
     </row>
     <row r="80" spans="2:15">
       <c r="B80" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="12"/>
-      <c r="K80" s="12"/>
-      <c r="L80" s="12"/>
       <c r="M80" s="5"/>
     </row>
     <row r="81" spans="2:14">
       <c r="B81" s="4"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="12"/>
-      <c r="K81" s="12"/>
-      <c r="L81" s="12"/>
       <c r="M81" s="5"/>
     </row>
     <row r="82" spans="2:14">
       <c r="B82" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="12"/>
-      <c r="K82" s="12"/>
-      <c r="L82" s="12"/>
       <c r="M82" s="5"/>
     </row>
     <row r="83" spans="2:14">
       <c r="B83" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
-      <c r="J83" s="12"/>
-      <c r="K83" s="12"/>
-      <c r="L83" s="12"/>
       <c r="M83" s="5"/>
     </row>
     <row r="84" spans="2:14">
       <c r="B84" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="12"/>
-      <c r="K84" s="12"/>
-      <c r="L84" s="12"/>
       <c r="M84" s="5"/>
     </row>
     <row r="85" spans="2:14">
       <c r="B85" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="12"/>
-      <c r="I85" s="12"/>
-      <c r="J85" s="12"/>
-      <c r="K85" s="12"/>
-      <c r="L85" s="12"/>
       <c r="M85" s="5"/>
     </row>
     <row r="86" spans="2:14">
       <c r="B86" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="12"/>
-      <c r="I86" s="12"/>
-      <c r="J86" s="12"/>
-      <c r="K86" s="12"/>
-      <c r="L86" s="12"/>
       <c r="M86" s="5"/>
     </row>
     <row r="87" spans="2:14">
@@ -6684,381 +6407,120 @@
       <c r="B91" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="12"/>
-      <c r="D91" s="12"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="12"/>
-      <c r="H91" s="12"/>
-      <c r="I91" s="12"/>
-      <c r="J91" s="12"/>
-      <c r="K91" s="12"/>
       <c r="L91" s="5"/>
     </row>
     <row r="92" spans="2:14">
       <c r="B92" s="4"/>
-      <c r="C92" s="12"/>
-      <c r="D92" s="12"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="12"/>
-      <c r="I92" s="12"/>
-      <c r="J92" s="12"/>
-      <c r="K92" s="12"/>
       <c r="L92" s="5"/>
     </row>
     <row r="93" spans="2:14">
       <c r="B93" s="4"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="12"/>
-      <c r="I93" s="12"/>
-      <c r="J93" s="12"/>
-      <c r="K93" s="12"/>
       <c r="L93" s="5"/>
     </row>
     <row r="94" spans="2:14">
       <c r="B94" s="4"/>
-      <c r="C94" s="12"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="12"/>
-      <c r="I94" s="12"/>
-      <c r="J94" s="12"/>
-      <c r="K94" s="12"/>
       <c r="L94" s="5"/>
     </row>
     <row r="95" spans="2:14">
       <c r="B95" s="4"/>
-      <c r="C95" s="12"/>
-      <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="12"/>
-      <c r="I95" s="12"/>
-      <c r="J95" s="12"/>
-      <c r="K95" s="12"/>
       <c r="L95" s="5"/>
     </row>
     <row r="96" spans="2:14">
       <c r="B96" s="4"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="12"/>
-      <c r="H96" s="12"/>
-      <c r="I96" s="12"/>
-      <c r="J96" s="12"/>
-      <c r="K96" s="12"/>
       <c r="L96" s="5"/>
     </row>
     <row r="97" spans="2:12">
       <c r="B97" s="4"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
-      <c r="E97" s="12"/>
-      <c r="F97" s="12"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="12"/>
-      <c r="I97" s="12"/>
-      <c r="J97" s="12"/>
-      <c r="K97" s="12"/>
       <c r="L97" s="5"/>
     </row>
     <row r="98" spans="2:12">
       <c r="B98" s="4"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="12"/>
-      <c r="I98" s="12"/>
-      <c r="J98" s="12"/>
-      <c r="K98" s="12"/>
       <c r="L98" s="5"/>
     </row>
     <row r="99" spans="2:12">
       <c r="B99" s="4"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="12"/>
-      <c r="I99" s="12"/>
-      <c r="J99" s="12"/>
-      <c r="K99" s="12"/>
       <c r="L99" s="5"/>
     </row>
     <row r="100" spans="2:12">
       <c r="B100" s="4"/>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="12"/>
-      <c r="K100" s="12"/>
       <c r="L100" s="5"/>
     </row>
     <row r="101" spans="2:12">
       <c r="B101" s="4"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="12"/>
-      <c r="I101" s="12"/>
-      <c r="J101" s="12"/>
-      <c r="K101" s="12"/>
       <c r="L101" s="5"/>
     </row>
     <row r="102" spans="2:12">
       <c r="B102" s="4"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="12"/>
-      <c r="I102" s="12"/>
-      <c r="J102" s="12"/>
-      <c r="K102" s="12"/>
       <c r="L102" s="5"/>
     </row>
     <row r="103" spans="2:12">
       <c r="B103" s="4"/>
-      <c r="C103" s="12"/>
-      <c r="D103" s="12"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
-      <c r="G103" s="12"/>
-      <c r="H103" s="12"/>
-      <c r="I103" s="12"/>
-      <c r="J103" s="12"/>
-      <c r="K103" s="12"/>
       <c r="L103" s="5"/>
     </row>
     <row r="104" spans="2:12">
       <c r="B104" s="4"/>
-      <c r="C104" s="12"/>
-      <c r="D104" s="12"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
-      <c r="G104" s="12"/>
-      <c r="H104" s="12"/>
-      <c r="I104" s="12"/>
-      <c r="J104" s="12"/>
-      <c r="K104" s="12"/>
       <c r="L104" s="5"/>
     </row>
     <row r="105" spans="2:12">
       <c r="B105" s="4"/>
-      <c r="C105" s="12"/>
-      <c r="D105" s="12"/>
-      <c r="E105" s="12"/>
-      <c r="F105" s="12"/>
-      <c r="G105" s="12"/>
-      <c r="H105" s="12"/>
-      <c r="I105" s="12"/>
-      <c r="J105" s="12"/>
-      <c r="K105" s="12"/>
       <c r="L105" s="5"/>
     </row>
     <row r="106" spans="2:12">
       <c r="B106" s="4"/>
-      <c r="C106" s="12"/>
-      <c r="D106" s="12"/>
-      <c r="E106" s="12"/>
-      <c r="F106" s="12"/>
-      <c r="G106" s="12"/>
-      <c r="H106" s="12"/>
-      <c r="I106" s="12"/>
-      <c r="J106" s="12"/>
-      <c r="K106" s="12"/>
       <c r="L106" s="5"/>
     </row>
     <row r="107" spans="2:12">
       <c r="B107" s="4"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
-      <c r="G107" s="12"/>
-      <c r="H107" s="12"/>
-      <c r="I107" s="12"/>
-      <c r="J107" s="12"/>
-      <c r="K107" s="12"/>
       <c r="L107" s="5"/>
     </row>
     <row r="108" spans="2:12">
       <c r="B108" s="4"/>
-      <c r="C108" s="12"/>
-      <c r="D108" s="12"/>
-      <c r="E108" s="12"/>
-      <c r="F108" s="12"/>
-      <c r="G108" s="12"/>
-      <c r="H108" s="12"/>
-      <c r="I108" s="12"/>
-      <c r="J108" s="12"/>
-      <c r="K108" s="12"/>
       <c r="L108" s="5"/>
     </row>
     <row r="109" spans="2:12">
       <c r="B109" s="4"/>
-      <c r="C109" s="12"/>
-      <c r="D109" s="12"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
-      <c r="G109" s="12"/>
-      <c r="H109" s="12"/>
-      <c r="I109" s="12"/>
-      <c r="J109" s="12"/>
-      <c r="K109" s="12"/>
       <c r="L109" s="5"/>
     </row>
     <row r="110" spans="2:12">
       <c r="B110" s="4"/>
-      <c r="C110" s="12"/>
-      <c r="D110" s="12"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="12"/>
-      <c r="G110" s="12"/>
-      <c r="H110" s="12"/>
-      <c r="I110" s="12"/>
-      <c r="J110" s="12"/>
-      <c r="K110" s="12"/>
       <c r="L110" s="5"/>
     </row>
     <row r="111" spans="2:12">
       <c r="B111" s="4"/>
-      <c r="C111" s="12"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
-      <c r="G111" s="12"/>
-      <c r="H111" s="12"/>
-      <c r="I111" s="12"/>
-      <c r="J111" s="12"/>
-      <c r="K111" s="12"/>
       <c r="L111" s="5"/>
     </row>
     <row r="112" spans="2:12">
       <c r="B112" s="4"/>
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
-      <c r="G112" s="12"/>
-      <c r="H112" s="12"/>
-      <c r="I112" s="12"/>
-      <c r="J112" s="12"/>
-      <c r="K112" s="12"/>
       <c r="L112" s="5"/>
     </row>
     <row r="113" spans="2:14">
       <c r="B113" s="4"/>
-      <c r="C113" s="12"/>
-      <c r="D113" s="12"/>
-      <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
-      <c r="G113" s="12"/>
-      <c r="H113" s="12"/>
-      <c r="I113" s="12"/>
-      <c r="J113" s="12"/>
-      <c r="K113" s="12"/>
       <c r="L113" s="5"/>
     </row>
     <row r="114" spans="2:14">
       <c r="B114" s="4"/>
-      <c r="C114" s="12"/>
-      <c r="D114" s="12"/>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
-      <c r="G114" s="12"/>
-      <c r="H114" s="12"/>
-      <c r="I114" s="12"/>
-      <c r="J114" s="12"/>
-      <c r="K114" s="12"/>
       <c r="L114" s="5"/>
     </row>
     <row r="115" spans="2:14">
       <c r="B115" s="4"/>
-      <c r="C115" s="12"/>
-      <c r="D115" s="12"/>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
-      <c r="G115" s="12"/>
-      <c r="H115" s="12"/>
-      <c r="I115" s="12"/>
-      <c r="J115" s="12"/>
-      <c r="K115" s="12"/>
       <c r="L115" s="5"/>
     </row>
     <row r="116" spans="2:14">
       <c r="B116" s="4"/>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
-      <c r="G116" s="12"/>
-      <c r="H116" s="12"/>
-      <c r="I116" s="12"/>
-      <c r="J116" s="12"/>
-      <c r="K116" s="12"/>
       <c r="L116" s="5"/>
     </row>
     <row r="117" spans="2:14">
       <c r="B117" s="4"/>
-      <c r="C117" s="12"/>
-      <c r="D117" s="12"/>
-      <c r="E117" s="12"/>
-      <c r="F117" s="12"/>
-      <c r="G117" s="12"/>
-      <c r="H117" s="12"/>
-      <c r="I117" s="12"/>
-      <c r="J117" s="12"/>
-      <c r="K117" s="12"/>
       <c r="L117" s="5"/>
     </row>
     <row r="118" spans="2:14">
       <c r="B118" s="4"/>
-      <c r="C118" s="12"/>
-      <c r="D118" s="12"/>
-      <c r="E118" s="12"/>
-      <c r="F118" s="12"/>
-      <c r="G118" s="12"/>
-      <c r="H118" s="12"/>
-      <c r="I118" s="12"/>
-      <c r="J118" s="12"/>
-      <c r="K118" s="12"/>
       <c r="L118" s="5"/>
     </row>
     <row r="119" spans="2:14">
       <c r="B119" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C119" s="12"/>
-      <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
-      <c r="G119" s="12"/>
-      <c r="H119" s="12"/>
-      <c r="I119" s="12"/>
-      <c r="J119" s="12"/>
-      <c r="K119" s="12"/>
       <c r="L119" s="5"/>
       <c r="M119" t="s">
         <v>23</v>
@@ -7071,15 +6533,6 @@
       <c r="B120" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C120" s="12"/>
-      <c r="D120" s="12"/>
-      <c r="E120" s="12"/>
-      <c r="F120" s="12"/>
-      <c r="G120" s="12"/>
-      <c r="H120" s="12"/>
-      <c r="I120" s="12"/>
-      <c r="J120" s="12"/>
-      <c r="K120" s="12"/>
       <c r="L120" s="5"/>
       <c r="N120" t="s">
         <v>93</v>
@@ -7087,106 +6540,34 @@
     </row>
     <row r="121" spans="2:14">
       <c r="B121" s="4"/>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
-      <c r="E121" s="12"/>
-      <c r="F121" s="12"/>
-      <c r="G121" s="12"/>
-      <c r="H121" s="12"/>
-      <c r="I121" s="12"/>
-      <c r="J121" s="12"/>
-      <c r="K121" s="12"/>
       <c r="L121" s="5"/>
     </row>
     <row r="122" spans="2:14">
       <c r="B122" s="4"/>
-      <c r="C122" s="12"/>
-      <c r="D122" s="12"/>
-      <c r="E122" s="12"/>
-      <c r="F122" s="12"/>
-      <c r="G122" s="12"/>
-      <c r="H122" s="12"/>
-      <c r="I122" s="12"/>
-      <c r="J122" s="12"/>
-      <c r="K122" s="12"/>
       <c r="L122" s="5"/>
     </row>
     <row r="123" spans="2:14">
       <c r="B123" s="4"/>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
-      <c r="E123" s="12"/>
-      <c r="F123" s="12"/>
-      <c r="G123" s="12"/>
-      <c r="H123" s="12"/>
-      <c r="I123" s="12"/>
-      <c r="J123" s="12"/>
-      <c r="K123" s="12"/>
       <c r="L123" s="5"/>
     </row>
     <row r="124" spans="2:14">
       <c r="B124" s="4"/>
-      <c r="C124" s="12"/>
-      <c r="D124" s="12"/>
-      <c r="E124" s="12"/>
-      <c r="F124" s="12"/>
-      <c r="G124" s="12"/>
-      <c r="H124" s="12"/>
-      <c r="I124" s="12"/>
-      <c r="J124" s="12"/>
-      <c r="K124" s="12"/>
       <c r="L124" s="5"/>
     </row>
     <row r="125" spans="2:14">
       <c r="B125" s="4"/>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
-      <c r="E125" s="12"/>
-      <c r="F125" s="12"/>
-      <c r="G125" s="12"/>
-      <c r="H125" s="12"/>
-      <c r="I125" s="12"/>
-      <c r="J125" s="12"/>
-      <c r="K125" s="12"/>
       <c r="L125" s="5"/>
     </row>
     <row r="126" spans="2:14">
       <c r="B126" s="4"/>
-      <c r="C126" s="12"/>
-      <c r="D126" s="12"/>
-      <c r="E126" s="12"/>
-      <c r="F126" s="12"/>
-      <c r="G126" s="12"/>
-      <c r="H126" s="12"/>
-      <c r="I126" s="12"/>
-      <c r="J126" s="12"/>
-      <c r="K126" s="12"/>
       <c r="L126" s="5"/>
     </row>
     <row r="127" spans="2:14">
       <c r="B127" s="4"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
-      <c r="E127" s="12"/>
-      <c r="F127" s="12"/>
-      <c r="G127" s="12"/>
-      <c r="H127" s="12"/>
-      <c r="I127" s="12"/>
-      <c r="J127" s="12"/>
-      <c r="K127" s="12"/>
       <c r="L127" s="5"/>
     </row>
     <row r="128" spans="2:14">
       <c r="B128" s="4"/>
-      <c r="C128" s="12"/>
-      <c r="D128" s="12"/>
-      <c r="E128" s="12"/>
-      <c r="F128" s="12"/>
-      <c r="G128" s="12"/>
-      <c r="H128" s="12"/>
-      <c r="I128" s="12"/>
-      <c r="J128" s="12"/>
-      <c r="K128" s="12"/>
       <c r="L128" s="5"/>
     </row>
     <row r="129" spans="2:12">
@@ -7221,119 +6602,38 @@
       <c r="B133" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C133" s="12"/>
-      <c r="D133" s="12"/>
-      <c r="E133" s="12"/>
-      <c r="F133" s="12"/>
-      <c r="G133" s="12"/>
-      <c r="H133" s="12"/>
-      <c r="I133" s="12"/>
-      <c r="J133" s="12"/>
-      <c r="K133" s="12"/>
       <c r="L133" s="5"/>
     </row>
     <row r="134" spans="2:12">
       <c r="B134" s="4"/>
-      <c r="C134" s="12"/>
-      <c r="D134" s="12"/>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12"/>
-      <c r="G134" s="12"/>
-      <c r="H134" s="12"/>
-      <c r="I134" s="12"/>
-      <c r="J134" s="12"/>
-      <c r="K134" s="12"/>
       <c r="L134" s="5"/>
     </row>
     <row r="135" spans="2:12">
       <c r="B135" s="4"/>
-      <c r="C135" s="12"/>
-      <c r="D135" s="12"/>
-      <c r="E135" s="12"/>
-      <c r="F135" s="12"/>
-      <c r="G135" s="12"/>
-      <c r="H135" s="12"/>
-      <c r="I135" s="12"/>
-      <c r="J135" s="12"/>
-      <c r="K135" s="12"/>
       <c r="L135" s="5"/>
     </row>
     <row r="136" spans="2:12">
       <c r="B136" s="4"/>
-      <c r="C136" s="12"/>
-      <c r="D136" s="12"/>
-      <c r="E136" s="12"/>
-      <c r="F136" s="12"/>
-      <c r="G136" s="12"/>
-      <c r="H136" s="12"/>
-      <c r="I136" s="12"/>
-      <c r="J136" s="12"/>
-      <c r="K136" s="12"/>
       <c r="L136" s="5"/>
     </row>
     <row r="137" spans="2:12">
       <c r="B137" s="4"/>
-      <c r="C137" s="12"/>
-      <c r="D137" s="12"/>
-      <c r="E137" s="12"/>
-      <c r="F137" s="12"/>
-      <c r="G137" s="12"/>
-      <c r="H137" s="12"/>
-      <c r="I137" s="12"/>
-      <c r="J137" s="12"/>
-      <c r="K137" s="12"/>
       <c r="L137" s="5"/>
     </row>
     <row r="138" spans="2:12">
       <c r="B138" s="4"/>
-      <c r="C138" s="12"/>
-      <c r="D138" s="12"/>
-      <c r="E138" s="12"/>
-      <c r="F138" s="12"/>
-      <c r="G138" s="12"/>
-      <c r="H138" s="12"/>
-      <c r="I138" s="12"/>
-      <c r="J138" s="12"/>
-      <c r="K138" s="12"/>
       <c r="L138" s="5"/>
     </row>
     <row r="139" spans="2:12">
       <c r="B139" s="4"/>
-      <c r="C139" s="12"/>
-      <c r="D139" s="12"/>
-      <c r="E139" s="12"/>
-      <c r="F139" s="12"/>
-      <c r="G139" s="12"/>
-      <c r="H139" s="12"/>
-      <c r="I139" s="12"/>
-      <c r="J139" s="12"/>
-      <c r="K139" s="12"/>
       <c r="L139" s="5"/>
     </row>
     <row r="140" spans="2:12">
       <c r="B140" s="4"/>
-      <c r="C140" s="12"/>
-      <c r="D140" s="12"/>
-      <c r="E140" s="12"/>
-      <c r="F140" s="12"/>
-      <c r="G140" s="12"/>
-      <c r="H140" s="12"/>
-      <c r="I140" s="12"/>
-      <c r="J140" s="12"/>
-      <c r="K140" s="12"/>
       <c r="L140" s="5"/>
     </row>
     <row r="141" spans="2:12">
       <c r="B141" s="4"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
-      <c r="E141" s="12"/>
-      <c r="F141" s="12"/>
-      <c r="G141" s="12"/>
-      <c r="H141" s="12"/>
-      <c r="I141" s="12"/>
-      <c r="J141" s="12"/>
-      <c r="K141" s="12"/>
       <c r="L141" s="5"/>
     </row>
     <row r="142" spans="2:12">
@@ -7375,142 +6675,42 @@
       <c r="B146" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C146" s="12"/>
-      <c r="D146" s="12"/>
-      <c r="E146" s="12"/>
-      <c r="F146" s="12"/>
-      <c r="G146" s="12"/>
-      <c r="H146" s="12"/>
-      <c r="I146" s="12"/>
-      <c r="J146" s="12"/>
-      <c r="K146" s="12"/>
-      <c r="L146" s="12"/>
       <c r="M146" s="5"/>
     </row>
     <row r="147" spans="2:15">
       <c r="B147" s="4"/>
-      <c r="C147" s="12"/>
-      <c r="D147" s="12"/>
-      <c r="E147" s="12"/>
-      <c r="F147" s="12"/>
-      <c r="G147" s="12"/>
-      <c r="H147" s="12"/>
-      <c r="I147" s="12"/>
-      <c r="J147" s="12"/>
-      <c r="K147" s="12"/>
-      <c r="L147" s="12"/>
       <c r="M147" s="5"/>
     </row>
     <row r="148" spans="2:15">
       <c r="B148" s="4"/>
-      <c r="C148" s="12"/>
-      <c r="D148" s="12"/>
-      <c r="E148" s="12"/>
-      <c r="F148" s="12"/>
-      <c r="G148" s="12"/>
-      <c r="H148" s="12"/>
-      <c r="I148" s="12"/>
-      <c r="J148" s="12"/>
-      <c r="K148" s="12"/>
-      <c r="L148" s="12"/>
       <c r="M148" s="5"/>
     </row>
     <row r="149" spans="2:15">
       <c r="B149" s="4"/>
-      <c r="C149" s="12"/>
-      <c r="D149" s="12"/>
-      <c r="E149" s="12"/>
-      <c r="F149" s="12"/>
-      <c r="G149" s="12"/>
-      <c r="H149" s="12"/>
-      <c r="I149" s="12"/>
-      <c r="J149" s="12"/>
-      <c r="K149" s="12"/>
-      <c r="L149" s="12"/>
       <c r="M149" s="5"/>
     </row>
     <row r="150" spans="2:15">
       <c r="B150" s="4"/>
-      <c r="C150" s="12"/>
-      <c r="D150" s="12"/>
-      <c r="E150" s="12"/>
-      <c r="F150" s="12"/>
-      <c r="G150" s="12"/>
-      <c r="H150" s="12"/>
-      <c r="I150" s="12"/>
-      <c r="J150" s="12"/>
-      <c r="K150" s="12"/>
-      <c r="L150" s="12"/>
       <c r="M150" s="5"/>
     </row>
     <row r="151" spans="2:15">
       <c r="B151" s="4"/>
-      <c r="C151" s="12"/>
-      <c r="D151" s="12"/>
-      <c r="E151" s="12"/>
-      <c r="F151" s="12"/>
-      <c r="G151" s="12"/>
-      <c r="H151" s="12"/>
-      <c r="I151" s="12"/>
-      <c r="J151" s="12"/>
-      <c r="K151" s="12"/>
-      <c r="L151" s="12"/>
       <c r="M151" s="5"/>
     </row>
     <row r="152" spans="2:15">
       <c r="B152" s="4"/>
-      <c r="C152" s="12"/>
-      <c r="D152" s="12"/>
-      <c r="E152" s="12"/>
-      <c r="F152" s="12"/>
-      <c r="G152" s="12"/>
-      <c r="H152" s="12"/>
-      <c r="I152" s="12"/>
-      <c r="J152" s="12"/>
-      <c r="K152" s="12"/>
-      <c r="L152" s="12"/>
       <c r="M152" s="5"/>
     </row>
     <row r="153" spans="2:15">
       <c r="B153" s="4"/>
-      <c r="C153" s="12"/>
-      <c r="D153" s="12"/>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12"/>
-      <c r="G153" s="12"/>
-      <c r="H153" s="12"/>
-      <c r="I153" s="12"/>
-      <c r="J153" s="12"/>
-      <c r="K153" s="12"/>
-      <c r="L153" s="12"/>
       <c r="M153" s="5"/>
     </row>
     <row r="154" spans="2:15">
       <c r="B154" s="4"/>
-      <c r="C154" s="12"/>
-      <c r="D154" s="12"/>
-      <c r="E154" s="12"/>
-      <c r="F154" s="12"/>
-      <c r="G154" s="12"/>
-      <c r="H154" s="12"/>
-      <c r="I154" s="12"/>
-      <c r="J154" s="12"/>
-      <c r="K154" s="12"/>
-      <c r="L154" s="12"/>
       <c r="M154" s="5"/>
     </row>
     <row r="155" spans="2:15">
       <c r="B155" s="4"/>
-      <c r="C155" s="12"/>
-      <c r="D155" s="12"/>
-      <c r="E155" s="12"/>
-      <c r="F155" s="12"/>
-      <c r="G155" s="12"/>
-      <c r="H155" s="12"/>
-      <c r="I155" s="12"/>
-      <c r="J155" s="12"/>
-      <c r="K155" s="12"/>
-      <c r="L155" s="12"/>
       <c r="M155" s="5"/>
     </row>
     <row r="156" spans="2:15">
@@ -7547,156 +6747,46 @@
       <c r="B160" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C160" s="12"/>
-      <c r="D160" s="12"/>
-      <c r="E160" s="12"/>
-      <c r="F160" s="12"/>
-      <c r="G160" s="12"/>
-      <c r="H160" s="12"/>
-      <c r="I160" s="12"/>
-      <c r="J160" s="12"/>
-      <c r="K160" s="12"/>
-      <c r="L160" s="12"/>
       <c r="M160" s="5"/>
     </row>
     <row r="161" spans="2:15">
       <c r="B161" s="4"/>
-      <c r="C161" s="12"/>
-      <c r="D161" s="12"/>
-      <c r="E161" s="12"/>
-      <c r="F161" s="12"/>
-      <c r="G161" s="12"/>
-      <c r="H161" s="12"/>
-      <c r="I161" s="12"/>
-      <c r="J161" s="12"/>
-      <c r="K161" s="12"/>
-      <c r="L161" s="12"/>
       <c r="M161" s="5"/>
     </row>
     <row r="162" spans="2:15">
       <c r="B162" s="4"/>
-      <c r="C162" s="12"/>
-      <c r="D162" s="12"/>
-      <c r="E162" s="12"/>
-      <c r="F162" s="12"/>
-      <c r="G162" s="12"/>
-      <c r="H162" s="12"/>
-      <c r="I162" s="12"/>
-      <c r="J162" s="12"/>
-      <c r="K162" s="12"/>
-      <c r="L162" s="12"/>
       <c r="M162" s="5"/>
     </row>
     <row r="163" spans="2:15">
       <c r="B163" s="4"/>
-      <c r="C163" s="12"/>
-      <c r="D163" s="12"/>
-      <c r="E163" s="12"/>
-      <c r="F163" s="12"/>
-      <c r="G163" s="12"/>
-      <c r="H163" s="12"/>
-      <c r="I163" s="12"/>
-      <c r="J163" s="12"/>
-      <c r="K163" s="12"/>
-      <c r="L163" s="12"/>
       <c r="M163" s="5"/>
     </row>
     <row r="164" spans="2:15">
       <c r="B164" s="4"/>
-      <c r="C164" s="12"/>
-      <c r="D164" s="12"/>
-      <c r="E164" s="12"/>
-      <c r="F164" s="12"/>
-      <c r="G164" s="12"/>
-      <c r="H164" s="12"/>
-      <c r="I164" s="12"/>
-      <c r="J164" s="12"/>
-      <c r="K164" s="12"/>
-      <c r="L164" s="12"/>
       <c r="M164" s="5"/>
     </row>
     <row r="165" spans="2:15">
       <c r="B165" s="4"/>
-      <c r="C165" s="12"/>
-      <c r="D165" s="12"/>
-      <c r="E165" s="12"/>
-      <c r="F165" s="12"/>
-      <c r="G165" s="12"/>
-      <c r="H165" s="12"/>
-      <c r="I165" s="12"/>
-      <c r="J165" s="12"/>
-      <c r="K165" s="12"/>
-      <c r="L165" s="12"/>
       <c r="M165" s="5"/>
     </row>
     <row r="166" spans="2:15">
       <c r="B166" s="4"/>
-      <c r="C166" s="12"/>
-      <c r="D166" s="12"/>
-      <c r="E166" s="12"/>
-      <c r="F166" s="12"/>
-      <c r="G166" s="12"/>
-      <c r="H166" s="12"/>
-      <c r="I166" s="12"/>
-      <c r="J166" s="12"/>
-      <c r="K166" s="12"/>
-      <c r="L166" s="12"/>
       <c r="M166" s="5"/>
     </row>
     <row r="167" spans="2:15">
       <c r="B167" s="4"/>
-      <c r="C167" s="12"/>
-      <c r="D167" s="12"/>
-      <c r="E167" s="12"/>
-      <c r="F167" s="12"/>
-      <c r="G167" s="12"/>
-      <c r="H167" s="12"/>
-      <c r="I167" s="12"/>
-      <c r="J167" s="12"/>
-      <c r="K167" s="12"/>
-      <c r="L167" s="12"/>
       <c r="M167" s="5"/>
     </row>
     <row r="168" spans="2:15">
       <c r="B168" s="4"/>
-      <c r="C168" s="12"/>
-      <c r="D168" s="12"/>
-      <c r="E168" s="12"/>
-      <c r="F168" s="12"/>
-      <c r="G168" s="12"/>
-      <c r="H168" s="12"/>
-      <c r="I168" s="12"/>
-      <c r="J168" s="12"/>
-      <c r="K168" s="12"/>
-      <c r="L168" s="12"/>
       <c r="M168" s="5"/>
     </row>
     <row r="169" spans="2:15">
       <c r="B169" s="4"/>
-      <c r="C169" s="12"/>
-      <c r="D169" s="12"/>
-      <c r="E169" s="12"/>
-      <c r="F169" s="12"/>
-      <c r="G169" s="12"/>
-      <c r="H169" s="12"/>
-      <c r="I169" s="12"/>
-      <c r="J169" s="12"/>
-      <c r="K169" s="12"/>
-      <c r="L169" s="12"/>
       <c r="M169" s="5"/>
     </row>
     <row r="170" spans="2:15">
       <c r="B170" s="4"/>
-      <c r="C170" s="12"/>
-      <c r="D170" s="12"/>
-      <c r="E170" s="12"/>
-      <c r="F170" s="12"/>
-      <c r="G170" s="12"/>
-      <c r="H170" s="12"/>
-      <c r="I170" s="12"/>
-      <c r="J170" s="12"/>
-      <c r="K170" s="12"/>
-      <c r="L170" s="12"/>
       <c r="M170" s="5"/>
       <c r="N170" t="s">
         <v>23</v>
@@ -7707,16 +6797,6 @@
     </row>
     <row r="171" spans="2:15">
       <c r="B171" s="4"/>
-      <c r="C171" s="12"/>
-      <c r="D171" s="12"/>
-      <c r="E171" s="12"/>
-      <c r="F171" s="12"/>
-      <c r="G171" s="12"/>
-      <c r="H171" s="12"/>
-      <c r="I171" s="12"/>
-      <c r="J171" s="12"/>
-      <c r="K171" s="12"/>
-      <c r="L171" s="12"/>
       <c r="M171" s="5"/>
     </row>
     <row r="172" spans="2:15">
@@ -7753,156 +6833,46 @@
       <c r="B176" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C176" s="12"/>
-      <c r="D176" s="12"/>
-      <c r="E176" s="12"/>
-      <c r="F176" s="12"/>
-      <c r="G176" s="12"/>
-      <c r="H176" s="12"/>
-      <c r="I176" s="12"/>
-      <c r="J176" s="12"/>
-      <c r="K176" s="12"/>
-      <c r="L176" s="12"/>
       <c r="M176" s="5"/>
     </row>
     <row r="177" spans="2:15">
       <c r="B177" s="4"/>
-      <c r="C177" s="12"/>
-      <c r="D177" s="12"/>
-      <c r="E177" s="12"/>
-      <c r="F177" s="12"/>
-      <c r="G177" s="12"/>
-      <c r="H177" s="12"/>
-      <c r="I177" s="12"/>
-      <c r="J177" s="12"/>
-      <c r="K177" s="12"/>
-      <c r="L177" s="12"/>
       <c r="M177" s="5"/>
     </row>
     <row r="178" spans="2:15">
       <c r="B178" s="4"/>
-      <c r="C178" s="12"/>
-      <c r="D178" s="12"/>
-      <c r="E178" s="12"/>
-      <c r="F178" s="12"/>
-      <c r="G178" s="12"/>
-      <c r="H178" s="12"/>
-      <c r="I178" s="12"/>
-      <c r="J178" s="12"/>
-      <c r="K178" s="12"/>
-      <c r="L178" s="12"/>
       <c r="M178" s="5"/>
     </row>
     <row r="179" spans="2:15">
       <c r="B179" s="4"/>
-      <c r="C179" s="12"/>
-      <c r="D179" s="12"/>
-      <c r="E179" s="12"/>
-      <c r="F179" s="12"/>
-      <c r="G179" s="12"/>
-      <c r="H179" s="12"/>
-      <c r="I179" s="12"/>
-      <c r="J179" s="12"/>
-      <c r="K179" s="12"/>
-      <c r="L179" s="12"/>
       <c r="M179" s="5"/>
     </row>
     <row r="180" spans="2:15">
       <c r="B180" s="4"/>
-      <c r="C180" s="12"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
-      <c r="G180" s="12"/>
-      <c r="H180" s="12"/>
-      <c r="I180" s="12"/>
-      <c r="J180" s="12"/>
-      <c r="K180" s="12"/>
-      <c r="L180" s="12"/>
       <c r="M180" s="5"/>
     </row>
     <row r="181" spans="2:15">
       <c r="B181" s="4"/>
-      <c r="C181" s="12"/>
-      <c r="D181" s="12"/>
-      <c r="E181" s="12"/>
-      <c r="F181" s="12"/>
-      <c r="G181" s="12"/>
-      <c r="H181" s="12"/>
-      <c r="I181" s="12"/>
-      <c r="J181" s="12"/>
-      <c r="K181" s="12"/>
-      <c r="L181" s="12"/>
       <c r="M181" s="5"/>
     </row>
     <row r="182" spans="2:15">
       <c r="B182" s="4"/>
-      <c r="C182" s="12"/>
-      <c r="D182" s="12"/>
-      <c r="E182" s="12"/>
-      <c r="F182" s="12"/>
-      <c r="G182" s="12"/>
-      <c r="H182" s="12"/>
-      <c r="I182" s="12"/>
-      <c r="J182" s="12"/>
-      <c r="K182" s="12"/>
-      <c r="L182" s="12"/>
       <c r="M182" s="5"/>
     </row>
     <row r="183" spans="2:15">
       <c r="B183" s="4"/>
-      <c r="C183" s="12"/>
-      <c r="D183" s="12"/>
-      <c r="E183" s="12"/>
-      <c r="F183" s="12"/>
-      <c r="G183" s="12"/>
-      <c r="H183" s="12"/>
-      <c r="I183" s="12"/>
-      <c r="J183" s="12"/>
-      <c r="K183" s="12"/>
-      <c r="L183" s="12"/>
       <c r="M183" s="5"/>
     </row>
     <row r="184" spans="2:15">
       <c r="B184" s="4"/>
-      <c r="C184" s="12"/>
-      <c r="D184" s="12"/>
-      <c r="E184" s="12"/>
-      <c r="F184" s="12"/>
-      <c r="G184" s="12"/>
-      <c r="H184" s="12"/>
-      <c r="I184" s="12"/>
-      <c r="J184" s="12"/>
-      <c r="K184" s="12"/>
-      <c r="L184" s="12"/>
       <c r="M184" s="5"/>
     </row>
     <row r="185" spans="2:15">
       <c r="B185" s="4"/>
-      <c r="C185" s="12"/>
-      <c r="D185" s="12"/>
-      <c r="E185" s="12"/>
-      <c r="F185" s="12"/>
-      <c r="G185" s="12"/>
-      <c r="H185" s="12"/>
-      <c r="I185" s="12"/>
-      <c r="J185" s="12"/>
-      <c r="K185" s="12"/>
-      <c r="L185" s="12"/>
       <c r="M185" s="5"/>
     </row>
     <row r="186" spans="2:15">
       <c r="B186" s="4"/>
-      <c r="C186" s="12"/>
-      <c r="D186" s="12"/>
-      <c r="E186" s="12"/>
-      <c r="F186" s="12"/>
-      <c r="G186" s="12"/>
-      <c r="H186" s="12"/>
-      <c r="I186" s="12"/>
-      <c r="J186" s="12"/>
-      <c r="K186" s="12"/>
-      <c r="L186" s="12"/>
       <c r="M186" s="5"/>
       <c r="N186" t="s">
         <v>23</v>
@@ -7945,170 +6915,50 @@
       <c r="B191" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C191" s="12"/>
-      <c r="D191" s="12"/>
-      <c r="E191" s="12"/>
-      <c r="F191" s="12"/>
-      <c r="G191" s="12"/>
-      <c r="H191" s="12"/>
-      <c r="I191" s="12"/>
-      <c r="J191" s="12"/>
-      <c r="K191" s="12"/>
-      <c r="L191" s="12"/>
       <c r="M191" s="5"/>
     </row>
     <row r="192" spans="2:15">
       <c r="B192" s="4"/>
-      <c r="C192" s="12"/>
-      <c r="D192" s="12"/>
-      <c r="E192" s="12"/>
-      <c r="F192" s="12"/>
-      <c r="G192" s="12"/>
-      <c r="H192" s="12"/>
-      <c r="I192" s="12"/>
-      <c r="J192" s="12"/>
-      <c r="K192" s="12"/>
-      <c r="L192" s="12"/>
       <c r="M192" s="5"/>
     </row>
     <row r="193" spans="2:15">
       <c r="B193" s="4"/>
-      <c r="C193" s="12"/>
-      <c r="D193" s="12"/>
-      <c r="E193" s="12"/>
-      <c r="F193" s="12"/>
-      <c r="G193" s="12"/>
-      <c r="H193" s="12"/>
-      <c r="I193" s="12"/>
-      <c r="J193" s="12"/>
-      <c r="K193" s="12"/>
-      <c r="L193" s="12"/>
       <c r="M193" s="5"/>
     </row>
     <row r="194" spans="2:15">
       <c r="B194" s="4"/>
-      <c r="C194" s="12"/>
-      <c r="D194" s="12"/>
-      <c r="E194" s="12"/>
-      <c r="F194" s="12"/>
-      <c r="G194" s="12"/>
-      <c r="H194" s="12"/>
-      <c r="I194" s="12"/>
-      <c r="J194" s="12"/>
-      <c r="K194" s="12"/>
-      <c r="L194" s="12"/>
       <c r="M194" s="5"/>
     </row>
     <row r="195" spans="2:15">
       <c r="B195" s="4"/>
-      <c r="C195" s="12"/>
-      <c r="D195" s="12"/>
-      <c r="E195" s="12"/>
-      <c r="F195" s="12"/>
-      <c r="G195" s="12"/>
-      <c r="H195" s="12"/>
-      <c r="I195" s="12"/>
-      <c r="J195" s="12"/>
-      <c r="K195" s="12"/>
-      <c r="L195" s="12"/>
       <c r="M195" s="5"/>
     </row>
     <row r="196" spans="2:15">
       <c r="B196" s="4"/>
-      <c r="C196" s="12"/>
-      <c r="D196" s="12"/>
-      <c r="E196" s="12"/>
-      <c r="F196" s="12"/>
-      <c r="G196" s="12"/>
-      <c r="H196" s="12"/>
-      <c r="I196" s="12"/>
-      <c r="J196" s="12"/>
-      <c r="K196" s="12"/>
-      <c r="L196" s="12"/>
       <c r="M196" s="5"/>
     </row>
     <row r="197" spans="2:15">
       <c r="B197" s="4"/>
-      <c r="C197" s="12"/>
-      <c r="D197" s="12"/>
-      <c r="E197" s="12"/>
-      <c r="F197" s="12"/>
-      <c r="G197" s="12"/>
-      <c r="H197" s="12"/>
-      <c r="I197" s="12"/>
-      <c r="J197" s="12"/>
-      <c r="K197" s="12"/>
-      <c r="L197" s="12"/>
       <c r="M197" s="5"/>
     </row>
     <row r="198" spans="2:15">
       <c r="B198" s="4"/>
-      <c r="C198" s="12"/>
-      <c r="D198" s="12"/>
-      <c r="E198" s="12"/>
-      <c r="F198" s="12"/>
-      <c r="G198" s="12"/>
-      <c r="H198" s="12"/>
-      <c r="I198" s="12"/>
-      <c r="J198" s="12"/>
-      <c r="K198" s="12"/>
-      <c r="L198" s="12"/>
       <c r="M198" s="5"/>
     </row>
     <row r="199" spans="2:15">
       <c r="B199" s="4"/>
-      <c r="C199" s="12"/>
-      <c r="D199" s="12"/>
-      <c r="E199" s="12"/>
-      <c r="F199" s="12"/>
-      <c r="G199" s="12"/>
-      <c r="H199" s="12"/>
-      <c r="I199" s="12"/>
-      <c r="J199" s="12"/>
-      <c r="K199" s="12"/>
-      <c r="L199" s="12"/>
       <c r="M199" s="5"/>
     </row>
     <row r="200" spans="2:15">
       <c r="B200" s="4"/>
-      <c r="C200" s="12"/>
-      <c r="D200" s="12"/>
-      <c r="E200" s="12"/>
-      <c r="F200" s="12"/>
-      <c r="G200" s="12"/>
-      <c r="H200" s="12"/>
-      <c r="I200" s="12"/>
-      <c r="J200" s="12"/>
-      <c r="K200" s="12"/>
-      <c r="L200" s="12"/>
       <c r="M200" s="5"/>
     </row>
     <row r="201" spans="2:15">
       <c r="B201" s="4"/>
-      <c r="C201" s="12"/>
-      <c r="D201" s="12"/>
-      <c r="E201" s="12"/>
-      <c r="F201" s="12"/>
-      <c r="G201" s="12"/>
-      <c r="H201" s="12"/>
-      <c r="I201" s="12"/>
-      <c r="J201" s="12"/>
-      <c r="K201" s="12"/>
-      <c r="L201" s="12"/>
       <c r="M201" s="5"/>
     </row>
     <row r="202" spans="2:15">
       <c r="B202" s="4"/>
-      <c r="C202" s="12"/>
-      <c r="D202" s="12"/>
-      <c r="E202" s="12"/>
-      <c r="F202" s="12"/>
-      <c r="G202" s="12"/>
-      <c r="H202" s="12"/>
-      <c r="I202" s="12"/>
-      <c r="J202" s="12"/>
-      <c r="K202" s="12"/>
-      <c r="L202" s="12"/>
       <c r="M202" s="5"/>
     </row>
     <row r="203" spans="2:15">
@@ -8151,254 +7001,74 @@
       <c r="B207" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C207" s="12"/>
-      <c r="D207" s="12"/>
-      <c r="E207" s="12"/>
-      <c r="F207" s="12"/>
-      <c r="G207" s="12"/>
-      <c r="H207" s="12"/>
-      <c r="I207" s="12"/>
-      <c r="J207" s="12"/>
-      <c r="K207" s="12"/>
-      <c r="L207" s="12"/>
       <c r="M207" s="5"/>
     </row>
     <row r="208" spans="2:15">
       <c r="B208" s="4"/>
-      <c r="C208" s="12"/>
-      <c r="D208" s="12"/>
-      <c r="E208" s="12"/>
-      <c r="F208" s="12"/>
-      <c r="G208" s="12"/>
-      <c r="H208" s="12"/>
-      <c r="I208" s="12"/>
-      <c r="J208" s="12"/>
-      <c r="K208" s="12"/>
-      <c r="L208" s="12"/>
       <c r="M208" s="5"/>
     </row>
     <row r="209" spans="2:13">
       <c r="B209" s="4"/>
-      <c r="C209" s="12"/>
-      <c r="D209" s="12"/>
-      <c r="E209" s="12"/>
-      <c r="F209" s="12"/>
-      <c r="G209" s="12"/>
-      <c r="H209" s="12"/>
-      <c r="I209" s="12"/>
-      <c r="J209" s="12"/>
-      <c r="K209" s="12"/>
-      <c r="L209" s="12"/>
       <c r="M209" s="5"/>
     </row>
     <row r="210" spans="2:13">
       <c r="B210" s="4"/>
-      <c r="C210" s="12"/>
-      <c r="D210" s="12"/>
-      <c r="E210" s="12"/>
-      <c r="F210" s="12"/>
-      <c r="G210" s="12"/>
-      <c r="H210" s="12"/>
-      <c r="I210" s="12"/>
-      <c r="J210" s="12"/>
-      <c r="K210" s="12"/>
-      <c r="L210" s="12"/>
       <c r="M210" s="5"/>
     </row>
     <row r="211" spans="2:13">
       <c r="B211" s="4"/>
-      <c r="C211" s="12"/>
-      <c r="D211" s="12"/>
-      <c r="E211" s="12"/>
-      <c r="F211" s="12"/>
-      <c r="G211" s="12"/>
-      <c r="H211" s="12"/>
-      <c r="I211" s="12"/>
-      <c r="J211" s="12"/>
-      <c r="K211" s="12"/>
-      <c r="L211" s="12"/>
       <c r="M211" s="5"/>
     </row>
     <row r="212" spans="2:13">
       <c r="B212" s="4"/>
-      <c r="C212" s="12"/>
-      <c r="D212" s="12"/>
-      <c r="E212" s="12"/>
-      <c r="F212" s="12"/>
-      <c r="G212" s="12"/>
-      <c r="H212" s="12"/>
-      <c r="I212" s="12"/>
-      <c r="J212" s="12"/>
-      <c r="K212" s="12"/>
-      <c r="L212" s="12"/>
       <c r="M212" s="5"/>
     </row>
     <row r="213" spans="2:13">
       <c r="B213" s="4"/>
-      <c r="C213" s="12"/>
-      <c r="D213" s="12"/>
-      <c r="E213" s="12"/>
-      <c r="F213" s="12"/>
-      <c r="G213" s="12"/>
-      <c r="H213" s="12"/>
-      <c r="I213" s="12"/>
-      <c r="J213" s="12"/>
-      <c r="K213" s="12"/>
-      <c r="L213" s="12"/>
       <c r="M213" s="5"/>
     </row>
     <row r="214" spans="2:13">
       <c r="B214" s="4"/>
-      <c r="C214" s="12"/>
-      <c r="D214" s="12"/>
-      <c r="E214" s="12"/>
-      <c r="F214" s="12"/>
-      <c r="G214" s="12"/>
-      <c r="H214" s="12"/>
-      <c r="I214" s="12"/>
-      <c r="J214" s="12"/>
-      <c r="K214" s="12"/>
-      <c r="L214" s="12"/>
       <c r="M214" s="5"/>
     </row>
     <row r="215" spans="2:13">
       <c r="B215" s="4"/>
-      <c r="C215" s="12"/>
-      <c r="D215" s="12"/>
-      <c r="E215" s="12"/>
-      <c r="F215" s="12"/>
-      <c r="G215" s="12"/>
-      <c r="H215" s="12"/>
-      <c r="I215" s="12"/>
-      <c r="J215" s="12"/>
-      <c r="K215" s="12"/>
-      <c r="L215" s="12"/>
       <c r="M215" s="5"/>
     </row>
     <row r="216" spans="2:13">
       <c r="B216" s="4"/>
-      <c r="C216" s="12"/>
-      <c r="D216" s="12"/>
-      <c r="E216" s="12"/>
-      <c r="F216" s="12"/>
-      <c r="G216" s="12"/>
-      <c r="H216" s="12"/>
-      <c r="I216" s="12"/>
-      <c r="J216" s="12"/>
-      <c r="K216" s="12"/>
-      <c r="L216" s="12"/>
       <c r="M216" s="5"/>
     </row>
     <row r="217" spans="2:13">
       <c r="B217" s="4"/>
-      <c r="C217" s="12"/>
-      <c r="D217" s="12"/>
-      <c r="E217" s="12"/>
-      <c r="F217" s="12"/>
-      <c r="G217" s="12"/>
-      <c r="H217" s="12"/>
-      <c r="I217" s="12"/>
-      <c r="J217" s="12"/>
-      <c r="K217" s="12"/>
-      <c r="L217" s="12"/>
       <c r="M217" s="5"/>
     </row>
     <row r="218" spans="2:13">
       <c r="B218" s="4"/>
-      <c r="C218" s="12"/>
-      <c r="D218" s="12"/>
-      <c r="E218" s="12"/>
-      <c r="F218" s="12"/>
-      <c r="G218" s="12"/>
-      <c r="H218" s="12"/>
-      <c r="I218" s="12"/>
-      <c r="J218" s="12"/>
-      <c r="K218" s="12"/>
-      <c r="L218" s="12"/>
       <c r="M218" s="5"/>
     </row>
     <row r="219" spans="2:13">
       <c r="B219" s="4"/>
-      <c r="C219" s="12"/>
-      <c r="D219" s="12"/>
-      <c r="E219" s="12"/>
-      <c r="F219" s="12"/>
-      <c r="G219" s="12"/>
-      <c r="H219" s="12"/>
-      <c r="I219" s="12"/>
-      <c r="J219" s="12"/>
-      <c r="K219" s="12"/>
-      <c r="L219" s="12"/>
       <c r="M219" s="5"/>
     </row>
     <row r="220" spans="2:13">
       <c r="B220" s="4"/>
-      <c r="C220" s="12"/>
-      <c r="D220" s="12"/>
-      <c r="E220" s="12"/>
-      <c r="F220" s="12"/>
-      <c r="G220" s="12"/>
-      <c r="H220" s="12"/>
-      <c r="I220" s="12"/>
-      <c r="J220" s="12"/>
-      <c r="K220" s="12"/>
-      <c r="L220" s="12"/>
       <c r="M220" s="5"/>
     </row>
     <row r="221" spans="2:13">
       <c r="B221" s="4"/>
-      <c r="C221" s="12"/>
-      <c r="D221" s="12"/>
-      <c r="E221" s="12"/>
-      <c r="F221" s="12"/>
-      <c r="G221" s="12"/>
-      <c r="H221" s="12"/>
-      <c r="I221" s="12"/>
-      <c r="J221" s="12"/>
-      <c r="K221" s="12"/>
-      <c r="L221" s="12"/>
       <c r="M221" s="5"/>
     </row>
     <row r="222" spans="2:13">
       <c r="B222" s="4"/>
-      <c r="C222" s="12"/>
-      <c r="D222" s="12"/>
-      <c r="E222" s="12"/>
-      <c r="F222" s="12"/>
-      <c r="G222" s="12"/>
-      <c r="H222" s="12"/>
-      <c r="I222" s="12"/>
-      <c r="J222" s="12"/>
-      <c r="K222" s="12"/>
-      <c r="L222" s="12"/>
       <c r="M222" s="5"/>
     </row>
     <row r="223" spans="2:13">
       <c r="B223" s="4"/>
-      <c r="C223" s="12"/>
-      <c r="D223" s="12"/>
-      <c r="E223" s="12"/>
-      <c r="F223" s="12"/>
-      <c r="G223" s="12"/>
-      <c r="H223" s="12"/>
-      <c r="I223" s="12"/>
-      <c r="J223" s="12"/>
-      <c r="K223" s="12"/>
-      <c r="L223" s="12"/>
       <c r="M223" s="5"/>
     </row>
     <row r="224" spans="2:13">
       <c r="B224" s="4"/>
-      <c r="C224" s="12"/>
-      <c r="D224" s="12"/>
-      <c r="E224" s="12"/>
-      <c r="F224" s="12"/>
-      <c r="G224" s="12"/>
-      <c r="H224" s="12"/>
-      <c r="I224" s="12"/>
-      <c r="J224" s="12"/>
-      <c r="K224" s="12"/>
-      <c r="L224" s="12"/>
       <c r="M224" s="5"/>
     </row>
     <row r="225" spans="2:15">
@@ -8441,16 +7111,6 @@
       <c r="B229" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C229" s="12"/>
-      <c r="D229" s="12"/>
-      <c r="E229" s="12"/>
-      <c r="F229" s="12"/>
-      <c r="G229" s="12"/>
-      <c r="H229" s="12"/>
-      <c r="I229" s="12"/>
-      <c r="J229" s="12"/>
-      <c r="K229" s="12"/>
-      <c r="L229" s="12"/>
       <c r="M229" s="5"/>
       <c r="O229" t="s">
         <v>105</v>
@@ -8458,170 +7118,50 @@
     </row>
     <row r="230" spans="2:15">
       <c r="B230" s="4"/>
-      <c r="C230" s="12"/>
-      <c r="D230" s="12"/>
-      <c r="E230" s="12"/>
-      <c r="F230" s="12"/>
-      <c r="G230" s="12"/>
-      <c r="H230" s="12"/>
-      <c r="I230" s="12"/>
-      <c r="J230" s="12"/>
-      <c r="K230" s="12"/>
-      <c r="L230" s="12"/>
       <c r="M230" s="5"/>
     </row>
     <row r="231" spans="2:15">
       <c r="B231" s="4"/>
-      <c r="C231" s="12"/>
-      <c r="D231" s="12"/>
-      <c r="E231" s="12"/>
-      <c r="F231" s="12"/>
-      <c r="G231" s="12"/>
-      <c r="H231" s="12"/>
-      <c r="I231" s="12"/>
-      <c r="J231" s="12"/>
-      <c r="K231" s="12"/>
-      <c r="L231" s="12"/>
       <c r="M231" s="5"/>
     </row>
     <row r="232" spans="2:15">
       <c r="B232" s="4"/>
-      <c r="C232" s="12"/>
-      <c r="D232" s="12"/>
-      <c r="E232" s="12"/>
-      <c r="F232" s="12"/>
-      <c r="G232" s="12"/>
-      <c r="H232" s="12"/>
-      <c r="I232" s="12"/>
-      <c r="J232" s="12"/>
-      <c r="K232" s="12"/>
-      <c r="L232" s="12"/>
       <c r="M232" s="5"/>
     </row>
     <row r="233" spans="2:15">
       <c r="B233" s="4"/>
-      <c r="C233" s="12"/>
-      <c r="D233" s="12"/>
-      <c r="E233" s="12"/>
-      <c r="F233" s="12"/>
-      <c r="G233" s="12"/>
-      <c r="H233" s="12"/>
-      <c r="I233" s="12"/>
-      <c r="J233" s="12"/>
-      <c r="K233" s="12"/>
-      <c r="L233" s="12"/>
       <c r="M233" s="5"/>
     </row>
     <row r="234" spans="2:15">
       <c r="B234" s="4"/>
-      <c r="C234" s="12"/>
-      <c r="D234" s="12"/>
-      <c r="E234" s="12"/>
-      <c r="F234" s="12"/>
-      <c r="G234" s="12"/>
-      <c r="H234" s="12"/>
-      <c r="I234" s="12"/>
-      <c r="J234" s="12"/>
-      <c r="K234" s="12"/>
-      <c r="L234" s="12"/>
       <c r="M234" s="5"/>
     </row>
     <row r="235" spans="2:15">
       <c r="B235" s="4"/>
-      <c r="C235" s="12"/>
-      <c r="D235" s="12"/>
-      <c r="E235" s="12"/>
-      <c r="F235" s="12"/>
-      <c r="G235" s="12"/>
-      <c r="H235" s="12"/>
-      <c r="I235" s="12"/>
-      <c r="J235" s="12"/>
-      <c r="K235" s="12"/>
-      <c r="L235" s="12"/>
       <c r="M235" s="5"/>
     </row>
     <row r="236" spans="2:15">
       <c r="B236" s="4"/>
-      <c r="C236" s="12"/>
-      <c r="D236" s="12"/>
-      <c r="E236" s="12"/>
-      <c r="F236" s="12"/>
-      <c r="G236" s="12"/>
-      <c r="H236" s="12"/>
-      <c r="I236" s="12"/>
-      <c r="J236" s="12"/>
-      <c r="K236" s="12"/>
-      <c r="L236" s="12"/>
       <c r="M236" s="5"/>
     </row>
     <row r="237" spans="2:15">
       <c r="B237" s="4"/>
-      <c r="C237" s="12"/>
-      <c r="D237" s="12"/>
-      <c r="E237" s="12"/>
-      <c r="F237" s="12"/>
-      <c r="G237" s="12"/>
-      <c r="H237" s="12"/>
-      <c r="I237" s="12"/>
-      <c r="J237" s="12"/>
-      <c r="K237" s="12"/>
-      <c r="L237" s="12"/>
       <c r="M237" s="5"/>
     </row>
     <row r="238" spans="2:15">
       <c r="B238" s="4"/>
-      <c r="C238" s="12"/>
-      <c r="D238" s="12"/>
-      <c r="E238" s="12"/>
-      <c r="F238" s="12"/>
-      <c r="G238" s="12"/>
-      <c r="H238" s="12"/>
-      <c r="I238" s="12"/>
-      <c r="J238" s="12"/>
-      <c r="K238" s="12"/>
-      <c r="L238" s="12"/>
       <c r="M238" s="5"/>
     </row>
     <row r="239" spans="2:15">
       <c r="B239" s="4"/>
-      <c r="C239" s="12"/>
-      <c r="D239" s="12"/>
-      <c r="E239" s="12"/>
-      <c r="F239" s="12"/>
-      <c r="G239" s="12"/>
-      <c r="H239" s="12"/>
-      <c r="I239" s="12"/>
-      <c r="J239" s="12"/>
-      <c r="K239" s="12"/>
-      <c r="L239" s="12"/>
       <c r="M239" s="5"/>
     </row>
     <row r="240" spans="2:15">
       <c r="B240" s="4"/>
-      <c r="C240" s="12"/>
-      <c r="D240" s="12"/>
-      <c r="E240" s="12"/>
-      <c r="F240" s="12"/>
-      <c r="G240" s="12"/>
-      <c r="H240" s="12"/>
-      <c r="I240" s="12"/>
-      <c r="J240" s="12"/>
-      <c r="K240" s="12"/>
-      <c r="L240" s="12"/>
       <c r="M240" s="5"/>
     </row>
     <row r="241" spans="2:19">
       <c r="B241" s="4"/>
-      <c r="C241" s="12"/>
-      <c r="D241" s="12"/>
-      <c r="E241" s="12"/>
-      <c r="F241" s="12"/>
-      <c r="G241" s="12"/>
-      <c r="H241" s="12"/>
-      <c r="I241" s="12"/>
-      <c r="J241" s="12"/>
-      <c r="K241" s="12"/>
-      <c r="L241" s="12"/>
       <c r="M241" s="5"/>
     </row>
     <row r="242" spans="2:19">
@@ -8664,308 +7204,68 @@
       <c r="B246" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C246" s="12"/>
-      <c r="D246" s="12"/>
-      <c r="E246" s="12"/>
-      <c r="F246" s="12"/>
-      <c r="G246" s="12"/>
-      <c r="H246" s="12"/>
-      <c r="I246" s="12"/>
-      <c r="J246" s="12"/>
-      <c r="K246" s="12"/>
-      <c r="L246" s="12"/>
-      <c r="M246" s="12"/>
-      <c r="N246" s="12"/>
-      <c r="O246" s="12"/>
-      <c r="P246" s="12"/>
-      <c r="Q246" s="12"/>
-      <c r="R246" s="12"/>
       <c r="S246" s="5"/>
     </row>
     <row r="247" spans="2:19">
       <c r="B247" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C247" s="12"/>
-      <c r="D247" s="12"/>
-      <c r="E247" s="12"/>
-      <c r="F247" s="12"/>
-      <c r="G247" s="12"/>
-      <c r="H247" s="12"/>
-      <c r="I247" s="12"/>
-      <c r="J247" s="12"/>
-      <c r="K247" s="12"/>
-      <c r="L247" s="12"/>
-      <c r="M247" s="12"/>
-      <c r="N247" s="12"/>
-      <c r="O247" s="12"/>
-      <c r="P247" s="12"/>
-      <c r="Q247" s="12"/>
-      <c r="R247" s="12"/>
       <c r="S247" s="5"/>
     </row>
     <row r="248" spans="2:19">
       <c r="B248" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C248" s="12"/>
-      <c r="D248" s="12"/>
-      <c r="E248" s="12"/>
-      <c r="F248" s="12"/>
-      <c r="G248" s="12"/>
-      <c r="H248" s="12"/>
-      <c r="I248" s="12"/>
-      <c r="J248" s="12"/>
-      <c r="K248" s="12"/>
-      <c r="L248" s="12"/>
-      <c r="M248" s="12"/>
-      <c r="N248" s="12"/>
-      <c r="O248" s="12"/>
-      <c r="P248" s="12"/>
-      <c r="Q248" s="12"/>
-      <c r="R248" s="12"/>
       <c r="S248" s="5"/>
     </row>
     <row r="249" spans="2:19">
-      <c r="B249" s="13" t="s">
+      <c r="B249" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C249" s="12"/>
-      <c r="D249" s="12"/>
-      <c r="E249" s="12"/>
-      <c r="F249" s="12"/>
-      <c r="G249" s="12"/>
-      <c r="H249" s="12"/>
-      <c r="I249" s="12"/>
-      <c r="J249" s="12"/>
-      <c r="K249" s="12"/>
-      <c r="L249" s="12"/>
-      <c r="M249" s="12"/>
-      <c r="N249" s="12"/>
-      <c r="O249" s="12"/>
-      <c r="P249" s="12"/>
-      <c r="Q249" s="12"/>
-      <c r="R249" s="12"/>
       <c r="S249" s="5"/>
     </row>
     <row r="250" spans="2:19">
       <c r="B250" s="4"/>
-      <c r="C250" s="12"/>
-      <c r="D250" s="12"/>
-      <c r="E250" s="12"/>
-      <c r="F250" s="12"/>
-      <c r="G250" s="12"/>
-      <c r="H250" s="12"/>
-      <c r="I250" s="12"/>
-      <c r="J250" s="12"/>
-      <c r="K250" s="12"/>
-      <c r="L250" s="12"/>
-      <c r="M250" s="12"/>
-      <c r="N250" s="12"/>
-      <c r="O250" s="12"/>
-      <c r="P250" s="12"/>
-      <c r="Q250" s="12"/>
-      <c r="R250" s="12"/>
       <c r="S250" s="5"/>
     </row>
     <row r="251" spans="2:19">
       <c r="B251" s="4"/>
-      <c r="C251" s="12"/>
-      <c r="D251" s="12"/>
-      <c r="E251" s="12"/>
-      <c r="F251" s="12"/>
-      <c r="G251" s="12"/>
-      <c r="H251" s="12"/>
-      <c r="I251" s="12"/>
-      <c r="J251" s="12"/>
-      <c r="K251" s="12"/>
-      <c r="L251" s="12"/>
-      <c r="M251" s="12"/>
-      <c r="N251" s="12"/>
-      <c r="O251" s="12"/>
-      <c r="P251" s="12"/>
-      <c r="Q251" s="12"/>
-      <c r="R251" s="12"/>
       <c r="S251" s="5"/>
     </row>
     <row r="252" spans="2:19">
       <c r="B252" s="4"/>
-      <c r="C252" s="12"/>
-      <c r="D252" s="12"/>
-      <c r="E252" s="12"/>
-      <c r="F252" s="12"/>
-      <c r="G252" s="12"/>
-      <c r="H252" s="12"/>
-      <c r="I252" s="12"/>
-      <c r="J252" s="12"/>
-      <c r="K252" s="12"/>
-      <c r="L252" s="12"/>
-      <c r="M252" s="12"/>
-      <c r="N252" s="12"/>
-      <c r="O252" s="12"/>
-      <c r="P252" s="12"/>
-      <c r="Q252" s="12"/>
-      <c r="R252" s="12"/>
       <c r="S252" s="5"/>
     </row>
     <row r="253" spans="2:19">
       <c r="B253" s="4"/>
-      <c r="C253" s="12"/>
-      <c r="D253" s="12"/>
-      <c r="E253" s="12"/>
-      <c r="F253" s="12"/>
-      <c r="G253" s="12"/>
-      <c r="H253" s="12"/>
-      <c r="I253" s="12"/>
-      <c r="J253" s="12"/>
-      <c r="K253" s="12"/>
-      <c r="L253" s="12"/>
-      <c r="M253" s="12"/>
-      <c r="N253" s="12"/>
-      <c r="O253" s="12"/>
-      <c r="P253" s="12"/>
-      <c r="Q253" s="12"/>
-      <c r="R253" s="12"/>
       <c r="S253" s="5"/>
     </row>
     <row r="254" spans="2:19">
       <c r="B254" s="4"/>
-      <c r="C254" s="12"/>
-      <c r="D254" s="12"/>
-      <c r="E254" s="12"/>
-      <c r="F254" s="12"/>
-      <c r="G254" s="12"/>
-      <c r="H254" s="12"/>
-      <c r="I254" s="12"/>
-      <c r="J254" s="12"/>
-      <c r="K254" s="12"/>
-      <c r="L254" s="12"/>
-      <c r="M254" s="12"/>
-      <c r="N254" s="12"/>
-      <c r="O254" s="12"/>
-      <c r="P254" s="12"/>
-      <c r="Q254" s="12"/>
-      <c r="R254" s="12"/>
       <c r="S254" s="5"/>
     </row>
     <row r="255" spans="2:19">
       <c r="B255" s="4"/>
-      <c r="C255" s="12"/>
-      <c r="D255" s="12"/>
-      <c r="E255" s="12"/>
-      <c r="F255" s="12"/>
-      <c r="G255" s="12"/>
-      <c r="H255" s="12"/>
-      <c r="I255" s="12"/>
-      <c r="J255" s="12"/>
-      <c r="K255" s="12"/>
-      <c r="L255" s="12"/>
-      <c r="M255" s="12"/>
-      <c r="N255" s="12"/>
-      <c r="O255" s="12"/>
-      <c r="P255" s="12"/>
-      <c r="Q255" s="12"/>
-      <c r="R255" s="12"/>
       <c r="S255" s="5"/>
     </row>
     <row r="256" spans="2:19">
       <c r="B256" s="4"/>
-      <c r="C256" s="12"/>
-      <c r="D256" s="12"/>
-      <c r="E256" s="12"/>
-      <c r="F256" s="12"/>
-      <c r="G256" s="12"/>
-      <c r="H256" s="12"/>
-      <c r="I256" s="12"/>
-      <c r="J256" s="12"/>
-      <c r="K256" s="12"/>
-      <c r="L256" s="12"/>
-      <c r="M256" s="12"/>
-      <c r="N256" s="12"/>
-      <c r="O256" s="12"/>
-      <c r="P256" s="12"/>
-      <c r="Q256" s="12"/>
-      <c r="R256" s="12"/>
       <c r="S256" s="5"/>
     </row>
     <row r="257" spans="2:21">
       <c r="B257" s="4"/>
-      <c r="C257" s="12"/>
-      <c r="D257" s="12"/>
-      <c r="E257" s="12"/>
-      <c r="F257" s="12"/>
-      <c r="G257" s="12"/>
-      <c r="H257" s="12"/>
-      <c r="I257" s="12"/>
-      <c r="J257" s="12"/>
-      <c r="K257" s="12"/>
-      <c r="L257" s="12"/>
-      <c r="M257" s="12"/>
-      <c r="N257" s="12"/>
-      <c r="O257" s="12"/>
-      <c r="P257" s="12"/>
-      <c r="Q257" s="12"/>
-      <c r="R257" s="12"/>
       <c r="S257" s="5"/>
     </row>
     <row r="258" spans="2:21">
       <c r="B258" s="4"/>
-      <c r="C258" s="12"/>
-      <c r="D258" s="12"/>
-      <c r="E258" s="12"/>
-      <c r="F258" s="12"/>
-      <c r="G258" s="12"/>
-      <c r="H258" s="12"/>
-      <c r="I258" s="12"/>
-      <c r="J258" s="12"/>
-      <c r="K258" s="12"/>
-      <c r="L258" s="12"/>
-      <c r="M258" s="12"/>
-      <c r="N258" s="12"/>
-      <c r="O258" s="12"/>
-      <c r="P258" s="12"/>
-      <c r="Q258" s="12"/>
-      <c r="R258" s="12"/>
       <c r="S258" s="5"/>
     </row>
     <row r="259" spans="2:21">
       <c r="B259" s="4"/>
-      <c r="C259" s="12"/>
-      <c r="D259" s="12"/>
-      <c r="E259" s="12"/>
-      <c r="F259" s="12"/>
-      <c r="G259" s="12"/>
-      <c r="H259" s="12"/>
-      <c r="I259" s="12"/>
-      <c r="J259" s="12"/>
-      <c r="K259" s="12"/>
-      <c r="L259" s="12"/>
-      <c r="M259" s="12"/>
-      <c r="N259" s="12"/>
-      <c r="O259" s="12"/>
-      <c r="P259" s="12"/>
-      <c r="Q259" s="12"/>
-      <c r="R259" s="12"/>
       <c r="S259" s="5"/>
     </row>
     <row r="260" spans="2:21">
       <c r="B260" s="4"/>
-      <c r="C260" s="12"/>
-      <c r="D260" s="12"/>
-      <c r="E260" s="12"/>
-      <c r="F260" s="12"/>
-      <c r="G260" s="12"/>
-      <c r="H260" s="12"/>
-      <c r="I260" s="12"/>
-      <c r="J260" s="12"/>
-      <c r="K260" s="12"/>
-      <c r="L260" s="12"/>
-      <c r="M260" s="12"/>
-      <c r="N260" s="12"/>
-      <c r="O260" s="12"/>
-      <c r="P260" s="12"/>
-      <c r="Q260" s="12"/>
-      <c r="R260" s="12"/>
       <c r="S260" s="5"/>
       <c r="T260" t="s">
         <v>23</v>
@@ -8976,282 +7276,58 @@
     </row>
     <row r="261" spans="2:21">
       <c r="B261" s="4"/>
-      <c r="C261" s="12"/>
-      <c r="D261" s="12"/>
-      <c r="E261" s="12"/>
-      <c r="F261" s="12"/>
-      <c r="G261" s="12"/>
-      <c r="H261" s="12"/>
-      <c r="I261" s="12"/>
-      <c r="J261" s="12"/>
-      <c r="K261" s="12"/>
-      <c r="L261" s="12"/>
-      <c r="M261" s="12"/>
-      <c r="N261" s="12"/>
-      <c r="O261" s="12"/>
-      <c r="P261" s="12"/>
-      <c r="Q261" s="12"/>
-      <c r="R261" s="12"/>
       <c r="S261" s="5"/>
     </row>
     <row r="262" spans="2:21">
       <c r="B262" s="4"/>
-      <c r="C262" s="12"/>
-      <c r="D262" s="12"/>
-      <c r="E262" s="12"/>
-      <c r="F262" s="12"/>
-      <c r="G262" s="12"/>
-      <c r="H262" s="12"/>
-      <c r="I262" s="12"/>
-      <c r="J262" s="12"/>
-      <c r="K262" s="12"/>
-      <c r="L262" s="12"/>
-      <c r="M262" s="12"/>
-      <c r="N262" s="12"/>
-      <c r="O262" s="12"/>
-      <c r="P262" s="12"/>
-      <c r="Q262" s="12"/>
-      <c r="R262" s="12"/>
       <c r="S262" s="5"/>
     </row>
     <row r="263" spans="2:21">
       <c r="B263" s="4"/>
-      <c r="C263" s="12"/>
-      <c r="D263" s="12"/>
-      <c r="E263" s="12"/>
-      <c r="F263" s="12"/>
-      <c r="G263" s="12"/>
-      <c r="H263" s="12"/>
-      <c r="I263" s="12"/>
-      <c r="J263" s="12"/>
-      <c r="K263" s="12"/>
-      <c r="L263" s="12"/>
-      <c r="M263" s="12"/>
-      <c r="N263" s="12"/>
-      <c r="O263" s="12"/>
-      <c r="P263" s="12"/>
-      <c r="Q263" s="12"/>
-      <c r="R263" s="12"/>
       <c r="S263" s="5"/>
     </row>
     <row r="264" spans="2:21">
       <c r="B264" s="4"/>
-      <c r="C264" s="12"/>
-      <c r="D264" s="12"/>
-      <c r="E264" s="12"/>
-      <c r="F264" s="12"/>
-      <c r="G264" s="12"/>
-      <c r="H264" s="12"/>
-      <c r="I264" s="12"/>
-      <c r="J264" s="12"/>
-      <c r="K264" s="12"/>
-      <c r="L264" s="12"/>
-      <c r="M264" s="12"/>
-      <c r="N264" s="12"/>
-      <c r="O264" s="12"/>
-      <c r="P264" s="12"/>
-      <c r="Q264" s="12"/>
-      <c r="R264" s="12"/>
       <c r="S264" s="5"/>
     </row>
     <row r="265" spans="2:21">
       <c r="B265" s="4"/>
-      <c r="C265" s="12"/>
-      <c r="D265" s="12"/>
-      <c r="E265" s="12"/>
-      <c r="F265" s="12"/>
-      <c r="G265" s="12"/>
-      <c r="H265" s="12"/>
-      <c r="I265" s="12"/>
-      <c r="J265" s="12"/>
-      <c r="K265" s="12"/>
-      <c r="L265" s="12"/>
-      <c r="M265" s="12"/>
-      <c r="N265" s="12"/>
-      <c r="O265" s="12"/>
-      <c r="P265" s="12"/>
-      <c r="Q265" s="12"/>
-      <c r="R265" s="12"/>
       <c r="S265" s="5"/>
     </row>
     <row r="266" spans="2:21">
       <c r="B266" s="4"/>
-      <c r="C266" s="12"/>
-      <c r="D266" s="12"/>
-      <c r="E266" s="12"/>
-      <c r="F266" s="12"/>
-      <c r="G266" s="12"/>
-      <c r="H266" s="12"/>
-      <c r="I266" s="12"/>
-      <c r="J266" s="12"/>
-      <c r="K266" s="12"/>
-      <c r="L266" s="12"/>
-      <c r="M266" s="12"/>
-      <c r="N266" s="12"/>
-      <c r="O266" s="12"/>
-      <c r="P266" s="12"/>
-      <c r="Q266" s="12"/>
-      <c r="R266" s="12"/>
       <c r="S266" s="5"/>
     </row>
     <row r="267" spans="2:21">
       <c r="B267" s="4"/>
-      <c r="C267" s="12"/>
-      <c r="D267" s="12"/>
-      <c r="E267" s="12"/>
-      <c r="F267" s="12"/>
-      <c r="G267" s="12"/>
-      <c r="H267" s="12"/>
-      <c r="I267" s="12"/>
-      <c r="J267" s="12"/>
-      <c r="K267" s="12"/>
-      <c r="L267" s="12"/>
-      <c r="M267" s="12"/>
-      <c r="N267" s="12"/>
-      <c r="O267" s="12"/>
-      <c r="P267" s="12"/>
-      <c r="Q267" s="12"/>
-      <c r="R267" s="12"/>
       <c r="S267" s="5"/>
     </row>
     <row r="268" spans="2:21">
       <c r="B268" s="4"/>
-      <c r="C268" s="12"/>
-      <c r="D268" s="12"/>
-      <c r="E268" s="12"/>
-      <c r="F268" s="12"/>
-      <c r="G268" s="12"/>
-      <c r="H268" s="12"/>
-      <c r="I268" s="12"/>
-      <c r="J268" s="12"/>
-      <c r="K268" s="12"/>
-      <c r="L268" s="12"/>
-      <c r="M268" s="12"/>
-      <c r="N268" s="12"/>
-      <c r="O268" s="12"/>
-      <c r="P268" s="12"/>
-      <c r="Q268" s="12"/>
-      <c r="R268" s="12"/>
       <c r="S268" s="5"/>
     </row>
     <row r="269" spans="2:21">
       <c r="B269" s="4"/>
-      <c r="C269" s="12"/>
-      <c r="D269" s="12"/>
-      <c r="E269" s="12"/>
-      <c r="F269" s="12"/>
-      <c r="G269" s="12"/>
-      <c r="H269" s="12"/>
-      <c r="I269" s="12"/>
-      <c r="J269" s="12"/>
-      <c r="K269" s="12"/>
-      <c r="L269" s="12"/>
-      <c r="M269" s="12"/>
-      <c r="N269" s="12"/>
-      <c r="O269" s="12"/>
-      <c r="P269" s="12"/>
-      <c r="Q269" s="12"/>
-      <c r="R269" s="12"/>
       <c r="S269" s="5"/>
     </row>
     <row r="270" spans="2:21">
       <c r="B270" s="4"/>
-      <c r="C270" s="12"/>
-      <c r="D270" s="12"/>
-      <c r="E270" s="12"/>
-      <c r="F270" s="12"/>
-      <c r="G270" s="12"/>
-      <c r="H270" s="12"/>
-      <c r="I270" s="12"/>
-      <c r="J270" s="12"/>
-      <c r="K270" s="12"/>
-      <c r="L270" s="12"/>
-      <c r="M270" s="12"/>
-      <c r="N270" s="12"/>
-      <c r="O270" s="12"/>
-      <c r="P270" s="12"/>
-      <c r="Q270" s="12"/>
-      <c r="R270" s="12"/>
       <c r="S270" s="5"/>
     </row>
     <row r="271" spans="2:21">
       <c r="B271" s="4"/>
-      <c r="C271" s="12"/>
-      <c r="D271" s="12"/>
-      <c r="E271" s="12"/>
-      <c r="F271" s="12"/>
-      <c r="G271" s="12"/>
-      <c r="H271" s="12"/>
-      <c r="I271" s="12"/>
-      <c r="J271" s="12"/>
-      <c r="K271" s="12"/>
-      <c r="L271" s="12"/>
-      <c r="M271" s="12"/>
-      <c r="N271" s="12"/>
-      <c r="O271" s="12"/>
-      <c r="P271" s="12"/>
-      <c r="Q271" s="12"/>
-      <c r="R271" s="12"/>
       <c r="S271" s="5"/>
     </row>
     <row r="272" spans="2:21">
       <c r="B272" s="4"/>
-      <c r="C272" s="12"/>
-      <c r="D272" s="12"/>
-      <c r="E272" s="12"/>
-      <c r="F272" s="12"/>
-      <c r="G272" s="12"/>
-      <c r="H272" s="12"/>
-      <c r="I272" s="12"/>
-      <c r="J272" s="12"/>
-      <c r="K272" s="12"/>
-      <c r="L272" s="12"/>
-      <c r="M272" s="12"/>
-      <c r="N272" s="12"/>
-      <c r="O272" s="12"/>
-      <c r="P272" s="12"/>
-      <c r="Q272" s="12"/>
-      <c r="R272" s="12"/>
       <c r="S272" s="5"/>
     </row>
     <row r="273" spans="2:19">
       <c r="B273" s="4"/>
-      <c r="C273" s="12"/>
-      <c r="D273" s="12"/>
-      <c r="E273" s="12"/>
-      <c r="F273" s="12"/>
-      <c r="G273" s="12"/>
-      <c r="H273" s="12"/>
-      <c r="I273" s="12"/>
-      <c r="J273" s="12"/>
-      <c r="K273" s="12"/>
-      <c r="L273" s="12"/>
-      <c r="M273" s="12"/>
-      <c r="N273" s="12"/>
-      <c r="O273" s="12"/>
-      <c r="P273" s="12"/>
-      <c r="Q273" s="12"/>
-      <c r="R273" s="12"/>
       <c r="S273" s="5"/>
     </row>
     <row r="274" spans="2:19">
       <c r="B274" s="4"/>
-      <c r="C274" s="12"/>
-      <c r="D274" s="12"/>
-      <c r="E274" s="12"/>
-      <c r="F274" s="12"/>
-      <c r="G274" s="12"/>
-      <c r="H274" s="12"/>
-      <c r="I274" s="12"/>
-      <c r="J274" s="12"/>
-      <c r="K274" s="12"/>
-      <c r="L274" s="12"/>
-      <c r="M274" s="12"/>
-      <c r="N274" s="12"/>
-      <c r="O274" s="12"/>
-      <c r="P274" s="12"/>
-      <c r="Q274" s="12"/>
-      <c r="R274" s="12"/>
       <c r="S274" s="5"/>
     </row>
     <row r="275" spans="2:19">
@@ -9279,4 +7355,660 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D94B178-AC33-4D3D-A569-38509326EA16}">
+  <dimension ref="B3:S78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:13">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="4"/>
+      <c r="D13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="4"/>
+      <c r="D18" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="4"/>
+      <c r="D19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="2:19">
+      <c r="B49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="2:19">
+      <c r="B50" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="2:19">
+      <c r="B51" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="2:19">
+      <c r="B52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="2:19">
+      <c r="B53" s="4"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="2:19">
+      <c r="B54" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="2:19">
+      <c r="B55" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="2:19">
+      <c r="B56" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="2:19">
+      <c r="B57" s="4"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="2:19">
+      <c r="B58" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="2:19">
+      <c r="B59" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="5"/>
+      <c r="K59" t="s">
+        <v>23</v>
+      </c>
+      <c r="L59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19">
+      <c r="B60" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="5"/>
+      <c r="L60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="2:19">
+      <c r="B61" s="7"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="9"/>
+    </row>
+    <row r="64" spans="2:19">
+      <c r="B64" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="2"/>
+      <c r="S64" s="3"/>
+    </row>
+    <row r="65" spans="2:19">
+      <c r="B65" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
+      <c r="S65" s="5"/>
+    </row>
+    <row r="66" spans="2:19">
+      <c r="B66" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="13"/>
+      <c r="O66" s="13"/>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="13"/>
+      <c r="S66" s="5"/>
+    </row>
+    <row r="67" spans="2:19">
+      <c r="B67" s="4"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13"/>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="13"/>
+      <c r="S67" s="5"/>
+    </row>
+    <row r="68" spans="2:19">
+      <c r="B68" s="4"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="13"/>
+      <c r="S68" s="5"/>
+    </row>
+    <row r="69" spans="2:19">
+      <c r="B69" s="4"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13"/>
+      <c r="O69" s="13"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="13"/>
+      <c r="S69" s="5"/>
+    </row>
+    <row r="70" spans="2:19">
+      <c r="B70" s="4"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13"/>
+      <c r="O70" s="13"/>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13"/>
+      <c r="R70" s="13"/>
+      <c r="S70" s="5"/>
+    </row>
+    <row r="71" spans="2:19">
+      <c r="B71" s="4"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13"/>
+      <c r="R71" s="13"/>
+      <c r="S71" s="5"/>
+    </row>
+    <row r="72" spans="2:19">
+      <c r="B72" s="4"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="13"/>
+      <c r="N72" s="13"/>
+      <c r="O72" s="13"/>
+      <c r="P72" s="13"/>
+      <c r="Q72" s="13"/>
+      <c r="R72" s="13"/>
+      <c r="S72" s="5"/>
+    </row>
+    <row r="73" spans="2:19">
+      <c r="B73" s="4"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="13"/>
+      <c r="Q73" s="13"/>
+      <c r="R73" s="13"/>
+      <c r="S73" s="5"/>
+    </row>
+    <row r="74" spans="2:19">
+      <c r="B74" s="4"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13"/>
+      <c r="O74" s="13"/>
+      <c r="P74" s="13"/>
+      <c r="Q74" s="13"/>
+      <c r="R74" s="13"/>
+      <c r="S74" s="5"/>
+    </row>
+    <row r="75" spans="2:19">
+      <c r="B75" s="4"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
+      <c r="O75" s="13"/>
+      <c r="P75" s="13"/>
+      <c r="Q75" s="13"/>
+      <c r="R75" s="13"/>
+      <c r="S75" s="5"/>
+    </row>
+    <row r="76" spans="2:19">
+      <c r="B76" s="4"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13"/>
+      <c r="O76" s="13"/>
+      <c r="P76" s="13"/>
+      <c r="Q76" s="13"/>
+      <c r="R76" s="13"/>
+      <c r="S76" s="5"/>
+    </row>
+    <row r="77" spans="2:19">
+      <c r="B77" s="4"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13"/>
+      <c r="O77" s="13"/>
+      <c r="P77" s="13"/>
+      <c r="Q77" s="13"/>
+      <c r="R77" s="13"/>
+      <c r="S77" s="5"/>
+    </row>
+    <row r="78" spans="2:19">
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="8"/>
+      <c r="N78" s="8"/>
+      <c r="O78" s="8"/>
+      <c r="P78" s="8"/>
+      <c r="Q78" s="8"/>
+      <c r="R78" s="8"/>
+      <c r="S78" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>